<commit_message>
updates to international migration calculations
</commit_message>
<xml_diff>
--- a/Output workbooks/internal_migration_local_authorities_statistics.xlsx
+++ b/Output workbooks/internal_migration_local_authorities_statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M.Lange\Documents\GitHub\urban-population-internal-migration\Output workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01FE7DCF-632B-4A61-B007-D135C3FD4A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED90C06-8D8C-4413-9FC5-F77CFAD3B824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inner London" sheetId="6" r:id="rId1"/>
@@ -15042,7 +15042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4ED0F5C-11F8-45B0-A356-872FD7FD6FF2}">
   <dimension ref="A1:AH195"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AH35" sqref="AH35"/>
     </sheetView>
   </sheetViews>
@@ -30640,7 +30640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BFEC768-C0E6-49AA-A200-2DB0973C7967}">
   <dimension ref="A1:AF47"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>

</xml_diff>